<commit_message>
Desplazamiento de todas las filas N posiciones desde un punto dado
</commit_message>
<xml_diff>
--- a/open_xml/excelTemplate.xlsx
+++ b/open_xml/excelTemplate.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\edgar\source\repos\open_xml\open_xml\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VisualStudio\open_xml\open_xml\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B513D31F-5AD1-417E-96E9-14C43A085630}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B981A9C1-03E5-4891-958F-4850CB6A6087}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{251F3AD6-E594-43C4-8F74-6383F175505A}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Template Tabla" sheetId="1" r:id="rId1"/>
+    <sheet name="Desplazar Filas" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Encabezado1</t>
   </si>
@@ -75,6 +76,36 @@
   </si>
   <si>
     <t>Aquí Va la Fecha</t>
+  </si>
+  <si>
+    <t>ENERO</t>
+  </si>
+  <si>
+    <t>FEBRERO</t>
+  </si>
+  <si>
+    <t>MARZO</t>
+  </si>
+  <si>
+    <t>JUNIO</t>
+  </si>
+  <si>
+    <t>JULIO</t>
+  </si>
+  <si>
+    <t>AGOSTO</t>
+  </si>
+  <si>
+    <t>SEPTIEMBRE</t>
+  </si>
+  <si>
+    <t>OCTUBRE</t>
+  </si>
+  <si>
+    <t>NOVIEMBRE</t>
+  </si>
+  <si>
+    <t>DICIEMBRE</t>
   </si>
 </sst>
 </file>
@@ -641,7 +672,7 @@
   <dimension ref="B1:L8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4:I4"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -785,4 +816,69 @@
     <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{014F4AF8-BAA3-4456-8D15-39AE2FD29EED}">
+  <dimension ref="A1:A10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>